<commit_message>
summaries grouped by drug category.
</commit_message>
<xml_diff>
--- a/tabular/contributed/drugs.xlsx
+++ b/tabular/contributed/drugs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17200" yWindow="8540" windowWidth="34040" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="16040" yWindow="8540" windowWidth="34040" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>glecaprevir</t>
   </si>
@@ -57,6 +57,15 @@
   </si>
   <si>
     <t>VOX</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>NS3/4A protease inhibitors</t>
+  </si>
+  <si>
+    <t>NS5A inhibitors</t>
   </si>
 </sst>
 </file>
@@ -392,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -401,46 +410,62 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates required to incorporate SOF table.
</commit_message>
<xml_diff>
--- a/tabular/contributed/drugs.xlsx
+++ b/tabular/contributed/drugs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16040" yWindow="8540" windowWidth="34040" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="15940" yWindow="8540" windowWidth="34040" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>glecaprevir</t>
   </si>
@@ -66,6 +66,42 @@
   </si>
   <si>
     <t>NS5A inhibitors</t>
+  </si>
+  <si>
+    <t>producer</t>
+  </si>
+  <si>
+    <t>researchCode</t>
+  </si>
+  <si>
+    <t>Abbvie</t>
+  </si>
+  <si>
+    <t>ABT-493</t>
+  </si>
+  <si>
+    <t>GS-5816</t>
+  </si>
+  <si>
+    <t>ABT-530</t>
+  </si>
+  <si>
+    <t>GS-9857</t>
+  </si>
+  <si>
+    <t>sofosbuvir</t>
+  </si>
+  <si>
+    <t>SOF</t>
+  </si>
+  <si>
+    <t>NS5B RNA polymerase inhibitors</t>
+  </si>
+  <si>
+    <t>GS-7977</t>
+  </si>
+  <si>
+    <t>Gilead Sciences</t>
   </si>
 </sst>
 </file>
@@ -401,7 +437,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -411,9 +447,10 @@
   <cols>
     <col min="1" max="1" width="21.1640625" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -423,8 +460,14 @@
       <c r="C1" t="s">
         <v>10</v>
       </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -434,8 +477,14 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -445,8 +494,14 @@
       <c r="C3" t="s">
         <v>12</v>
       </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -456,8 +511,14 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -466,6 +527,29 @@
       </c>
       <c r="C5" t="s">
         <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
various updates for dealing with subgenomic sequence data.
</commit_message>
<xml_diff>
--- a/tabular/contributed/drugs.xlsx
+++ b/tabular/contributed/drugs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15940" yWindow="8540" windowWidth="34040" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="15740" yWindow="8540" windowWidth="34040" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>glecaprevir</t>
   </si>
@@ -102,6 +102,18 @@
   </si>
   <si>
     <t>Gilead Sciences</t>
+  </si>
+  <si>
+    <t>NS3</t>
+  </si>
+  <si>
+    <t>NS5A</t>
+  </si>
+  <si>
+    <t>NS5B</t>
+  </si>
+  <si>
+    <t>featureRequiringCoverage</t>
   </si>
 </sst>
 </file>
@@ -437,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -450,7 +462,7 @@
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -466,8 +478,11 @@
       <c r="E1" t="s">
         <v>14</v>
       </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -483,8 +498,11 @@
       <c r="E2" t="s">
         <v>16</v>
       </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -500,8 +518,11 @@
       <c r="E3" t="s">
         <v>17</v>
       </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -517,8 +538,11 @@
       <c r="E4" t="s">
         <v>18</v>
       </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -534,8 +558,11 @@
       <c r="E5" t="s">
         <v>19</v>
       </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -550,6 +577,9 @@
       </c>
       <c r="E6" t="s">
         <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"insufficient coverage" criteria updated, now based on coverage of relevant locations. implementation currently limited to FASTA processing.
</commit_message>
<xml_diff>
--- a/tabular/contributed/drugs.xlsx
+++ b/tabular/contributed/drugs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21620" yWindow="9960" windowWidth="34040" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="15720" yWindow="9960" windowWidth="34040" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>id</t>
   </si>
@@ -89,27 +89,18 @@
     <t>MK-8742</t>
   </si>
   <si>
-    <t>NS5A</t>
-  </si>
-  <si>
     <t>producer</t>
   </si>
   <si>
     <t>researchCode</t>
   </si>
   <si>
-    <t>featureRequiringCoverage</t>
-  </si>
-  <si>
     <t>Abbvie</t>
   </si>
   <si>
     <t>ABT-493</t>
   </si>
   <si>
-    <t>NS3</t>
-  </si>
-  <si>
     <t>Gilead Sciences</t>
   </si>
   <si>
@@ -123,9 +114,6 @@
   </si>
   <si>
     <t>GS-7977</t>
-  </si>
-  <si>
-    <t>NS5B</t>
   </si>
 </sst>
 </file>
@@ -484,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -497,7 +485,7 @@
     <col min="4" max="4" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -508,16 +496,13 @@
         <v>14</v>
       </c>
       <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -528,16 +513,13 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -553,11 +535,8 @@
       <c r="E3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -568,16 +547,13 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -588,16 +564,13 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -608,16 +581,13 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
         <v>27</v>
       </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -628,19 +598,16 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
     </row>

</xml_diff>

<commit_message>
initial work on grazoprevir.
</commit_message>
<xml_diff>
--- a/tabular/contributed/drugs.xlsx
+++ b/tabular/contributed/drugs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15720" yWindow="9960" windowWidth="34040" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="8860" yWindow="8320" windowWidth="34040" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>id</t>
   </si>
@@ -135,6 +135,15 @@
   </si>
   <si>
     <t>BMS-790052</t>
+  </si>
+  <si>
+    <t>grazoprevir</t>
+  </si>
+  <si>
+    <t>GZR</t>
+  </si>
+  <si>
+    <t>MK-5172</t>
   </si>
 </sst>
 </file>
@@ -659,6 +668,23 @@
         <v>35</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>

</xml_diff>

<commit_message>
preparatory work for PrOD combination tables.
</commit_message>
<xml_diff>
--- a/tabular/contributed/drugs.xlsx
+++ b/tabular/contributed/drugs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8860" yWindow="8320" windowWidth="34040" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="14480" yWindow="7460" windowWidth="34040" windowHeight="16880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
   <si>
     <t>id</t>
   </si>
@@ -144,6 +144,33 @@
   </si>
   <si>
     <t>MK-5172</t>
+  </si>
+  <si>
+    <t>ombitasvir</t>
+  </si>
+  <si>
+    <t>paritaprevir</t>
+  </si>
+  <si>
+    <t>dasabuvir</t>
+  </si>
+  <si>
+    <t>ABT-267</t>
+  </si>
+  <si>
+    <t>OBV</t>
+  </si>
+  <si>
+    <t>PTV</t>
+  </si>
+  <si>
+    <t>DSV</t>
+  </si>
+  <si>
+    <t>ABT-450</t>
+  </si>
+  <si>
+    <t>ABT-333</t>
   </si>
 </sst>
 </file>
@@ -505,7 +532,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -685,6 +712,57 @@
         <v>38</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+    </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>

</xml_diff>